<commit_message>
Fix adjustment when education >20
</commit_message>
<xml_diff>
--- a/data-raw/neuronorma.xlsx
+++ b/data-raw/neuronorma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/GitHub/neuronorma/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7835C6BD-0FEF-9D49-91B5-15C51E84CD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763E5EEF-6706-974F-AEFB-90853B8CCB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Age" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="487">
   <si>
     <t>SS</t>
   </si>
@@ -1494,6 +1494,9 @@
   </si>
   <si>
     <t>ROCF_DR_Acc</t>
+  </si>
+  <si>
+    <t>&gt;20</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1C2EBB-8362-9645-B110-F28D92007116}">
   <dimension ref="A1:F188"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -4895,8 +4898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD1ADC0-39C1-5146-853B-75F39D4F50C6}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5375,8 +5378,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>20</v>
+      <c r="A23" s="3" t="s">
+        <v>486</v>
       </c>
       <c r="B23" s="3">
         <v>-3</v>
@@ -5411,7 +5414,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6770,9 +6773,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>20</v>
+    <row r="15" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>486</v>
       </c>
       <c r="B15" s="2">
         <v>-3</v>
@@ -6884,7 +6887,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AG30" sqref="AG30"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8243,9 +8246,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>20</v>
+    <row r="15" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>486</v>
       </c>
       <c r="B15" s="2">
         <v>-2</v>

</xml_diff>